<commit_message>
Set up file to begin creating training data for the 23andMe union dataset
</commit_message>
<xml_diff>
--- a/Data/PRS313.xlsx
+++ b/Data/PRS313.xlsx
@@ -1600,7 +1600,7 @@
     <col min="13" max="13" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1711,7 +1711,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1896,7 +1896,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -2007,7 +2007,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2229,7 +2229,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -2303,7 +2303,7 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -2340,7 +2340,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="5" t="s">
         <v>41</v>
       </c>

</xml_diff>